<commit_message>
added points performance calculation, tidying up dataframe cleaning
</commit_message>
<xml_diff>
--- a/credit_cards_test.xlsx
+++ b/credit_cards_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Endicott/dev/Software/swipe-rewards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741024A8-AABC-0847-9E01-380F483E5470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7FFDFB-6981-6C40-B8FA-3A23F910404E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="600" windowWidth="26760" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="credit_cards.csv" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Cards</t>
   </si>
@@ -96,27 +96,9 @@
     <t>Points Currency</t>
   </si>
   <si>
-    <t>UR</t>
-  </si>
-  <si>
-    <t>AMZN</t>
-  </si>
-  <si>
     <t>CASH</t>
   </si>
   <si>
-    <t>VR</t>
-  </si>
-  <si>
-    <t>COSTCO</t>
-  </si>
-  <si>
-    <t>TY</t>
-  </si>
-  <si>
-    <t>MR</t>
-  </si>
-  <si>
     <t>2019-12-01</t>
   </si>
   <si>
@@ -172,6 +154,45 @@
   </si>
   <si>
     <t>Bank of America Card 1</t>
+  </si>
+  <si>
+    <t>Issuer</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>American Express</t>
+  </si>
+  <si>
+    <t>Capital One</t>
+  </si>
+  <si>
+    <t>Barclays</t>
+  </si>
+  <si>
+    <t>Citi</t>
+  </si>
+  <si>
+    <t>Bank of America</t>
+  </si>
+  <si>
+    <t>UR (Chase)</t>
+  </si>
+  <si>
+    <t>AMZN (Amazon)</t>
+  </si>
+  <si>
+    <t>VR (CapOne)</t>
+  </si>
+  <si>
+    <t>COST (Costco)</t>
+  </si>
+  <si>
+    <t>TY (Citi)</t>
+  </si>
+  <si>
+    <t>MR (AMEX)</t>
   </si>
 </sst>
 </file>
@@ -601,384 +622,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>50000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>95</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>50000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>95</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>150</v>
+      </c>
+      <c r="G9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>95</v>
+      </c>
+      <c r="J9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10">
+        <v>50000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>150</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>50000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>95</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>500</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8">
-        <v>50000</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8">
-        <v>95</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9">
-        <v>150</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9">
-        <v>95</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10">
-        <v>50000</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10">
-        <v>150</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11">
-        <v>500</v>
-      </c>
-      <c r="F11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12">
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
         <v>200</v>
       </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
       <c r="G12" t="s">
         <v>6</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="2"/>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated column name in test excel file, added example screenshot of gui and example output file
</commit_message>
<xml_diff>
--- a/credit_cards_test.xlsx
+++ b/credit_cards_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Endicott/dev/Software/swipe-rewards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7FFDFB-6981-6C40-B8FA-3A23F910404E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5125004B-E445-6640-B691-97CD4BA2673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="credit_cards.csv" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
-  <si>
-    <t>Cards</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Date Opened</t>
   </si>
@@ -51,18 +48,9 @@
     <t>2016-08-20</t>
   </si>
   <si>
-    <t>2014-01-16</t>
-  </si>
-  <si>
-    <t>2014-04-23</t>
-  </si>
-  <si>
     <t>2018-05-29</t>
   </si>
   <si>
-    <t>2014-10-26</t>
-  </si>
-  <si>
     <t>2011-09-22</t>
   </si>
   <si>
@@ -193,6 +181,21 @@
   </si>
   <si>
     <t>MR (AMEX)</t>
+  </si>
+  <si>
+    <t>Card Name</t>
+  </si>
+  <si>
+    <t>2021-04-23</t>
+  </si>
+  <si>
+    <t>2021-01-16</t>
+  </si>
+  <si>
+    <t>2021-05-23</t>
+  </si>
+  <si>
+    <t>2021-10-26</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,45 +646,45 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
         <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -689,27 +692,27 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -717,289 +720,289 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>50000</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5">
         <v>95</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8">
         <v>50000</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8">
         <v>95</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>150</v>
       </c>
       <c r="G9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I9">
         <v>95</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F10">
         <v>50000</v>
       </c>
       <c r="G10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10">
         <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F11">
         <v>500</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F12">
         <v>200</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>